<commit_message>
Updated Excel files for 4.7.0
</commit_message>
<xml_diff>
--- a/public/excel-files/atlas-matrices.xlsx
+++ b/public/excel-files/atlas-matrices.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="105">
   <si>
     <t>Reconnaissance</t>
   </si>
@@ -100,9 +100,15 @@
     <t>Poison Training Data</t>
   </si>
   <si>
+    <t>Publish Hallucinated Entities</t>
+  </si>
+  <si>
     <t>Publish Poisoned Datasets</t>
   </si>
   <si>
+    <t>Publish Poisoned Models</t>
+  </si>
+  <si>
     <t>Consumer Hardware</t>
   </si>
   <si>
@@ -151,7 +157,7 @@
     <t>Data</t>
   </si>
   <si>
-    <t>GPU Hardware</t>
+    <t>Hardware</t>
   </si>
   <si>
     <t>ML Software</t>
@@ -163,12 +169,12 @@
     <t>Spearphishing via Social Engineering LLM</t>
   </si>
   <si>
+    <t>AI Model Inference API Access</t>
+  </si>
+  <si>
     <t>Full ML Model Access</t>
   </si>
   <si>
-    <t>ML Model Inference API Access</t>
-  </si>
-  <si>
     <t>ML-Enabled Product or Service</t>
   </si>
   <si>
@@ -190,6 +196,9 @@
     <t>Backdoor ML Model</t>
   </si>
   <si>
+    <t>LLM Prompt Self-Replication</t>
+  </si>
+  <si>
     <t>Inject Payload</t>
   </si>
   <si>
@@ -202,6 +211,12 @@
     <t>Unsecured Credentials</t>
   </si>
   <si>
+    <t>Discover AI Model Outputs</t>
+  </si>
+  <si>
+    <t>Discover LLM Hallucinations</t>
+  </si>
+  <si>
     <t>Discover ML Artifacts</t>
   </si>
   <si>
@@ -214,6 +229,12 @@
     <t>LLM Meta Prompt Extraction</t>
   </si>
   <si>
+    <t>Domains</t>
+  </si>
+  <si>
+    <t>Physical Countermeasures</t>
+  </si>
+  <si>
     <t>Data from Information Repositories</t>
   </si>
   <si>
@@ -280,6 +301,9 @@
     <t>Denial of ML Service</t>
   </si>
   <si>
+    <t>Erode Dataset Integrity</t>
+  </si>
+  <si>
     <t>Erode ML Model Integrity</t>
   </si>
   <si>
@@ -287,6 +311,9 @@
   </si>
   <si>
     <t>Spamming ML System with Chaff Data</t>
+  </si>
+  <si>
+    <t>Malicious Package</t>
   </si>
   <si>
     <t>Financial Harm</t>
@@ -697,7 +724,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X12"/>
+  <dimension ref="A1:Y13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -718,17 +745,20 @@
     <col min="13" max="13" width="20.7109375" style="2" customWidth="1"/>
     <col min="14" max="14" width="20.7109375" style="1" customWidth="1"/>
     <col min="15" max="15" width="20.7109375" style="2" customWidth="1"/>
-    <col min="16" max="18" width="20.7109375" customWidth="1"/>
-    <col min="19" max="19" width="20.7109375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="20.7109375" style="2" customWidth="1"/>
-    <col min="21" max="21" width="20.7109375" style="1" customWidth="1"/>
-    <col min="22" max="22" width="20.7109375" style="2" customWidth="1"/>
-    <col min="23" max="23" width="20.7109375" style="1" customWidth="1"/>
-    <col min="24" max="24" width="20.7109375" style="2" customWidth="1"/>
-    <col min="25" max="25" width="20.7109375" customWidth="1"/>
+    <col min="16" max="16" width="20.7109375" customWidth="1"/>
+    <col min="17" max="17" width="20.7109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="20.7109375" style="2" customWidth="1"/>
+    <col min="19" max="19" width="20.7109375" customWidth="1"/>
+    <col min="20" max="20" width="20.7109375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="20.7109375" style="2" customWidth="1"/>
+    <col min="22" max="22" width="20.7109375" style="1" customWidth="1"/>
+    <col min="23" max="23" width="20.7109375" style="2" customWidth="1"/>
+    <col min="24" max="24" width="20.7109375" style="1" customWidth="1"/>
+    <col min="25" max="25" width="20.7109375" style="2" customWidth="1"/>
+    <col min="26" max="26" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -763,26 +793,27 @@
       <c r="P1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3"/>
+      <c r="S1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="3"/>
+      <c r="V1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="3"/>
+      <c r="X1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:25">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -790,99 +821,102 @@
         <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="P2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="S2" t="s">
+        <v>73</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="U2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="Q2" t="s">
-        <v>62</v>
-      </c>
-      <c r="R2" t="s">
-        <v>66</v>
-      </c>
-      <c r="S2" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>86</v>
+      <c r="V2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:25">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="J3" s="5"/>
       <c r="K3" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q3" t="s">
         <v>63</v>
       </c>
-      <c r="R3" t="s">
-        <v>67</v>
-      </c>
-      <c r="S3" s="5"/>
-      <c r="T3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="U3" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>87</v>
+      <c r="Q3" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="S3" t="s">
+        <v>74</v>
+      </c>
+      <c r="T3" s="5"/>
+      <c r="U3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:25">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -890,104 +924,108 @@
         <v>23</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>64</v>
-      </c>
-      <c r="R4" t="s">
-        <v>68</v>
-      </c>
-      <c r="S4" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="T4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U4" s="5"/>
-      <c r="V4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>88</v>
+      <c r="S4" t="s">
+        <v>75</v>
+      </c>
+      <c r="T4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V4" s="5"/>
+      <c r="W4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:25">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="L5" s="5"/>
       <c r="M5" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N5" s="5"/>
       <c r="O5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>65</v>
-      </c>
-      <c r="S5" s="5"/>
-      <c r="T5" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="U5" s="5"/>
-      <c r="V5" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="T5" s="5"/>
+      <c r="U5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="V5" s="5"/>
+      <c r="W5" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:25">
       <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
@@ -998,32 +1036,32 @@
         <v>24</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S6" s="5"/>
-      <c r="T6" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="W6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="T6" s="5"/>
+      <c r="U6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="V6" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="X6" s="2" t="s">
-        <v>91</v>
+      <c r="X6" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:25">
       <c r="A7" s="5"/>
       <c r="B7" s="2" t="s">
         <v>20</v>
@@ -1033,21 +1071,29 @@
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="S7" s="5"/>
-      <c r="T7" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="W7" s="5"/>
-      <c r="X7" s="2" t="s">
-        <v>92</v>
+        <v>47</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="T7" s="5"/>
+      <c r="U7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="X7" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:25">
       <c r="A8" s="5"/>
       <c r="B8" s="2" t="s">
         <v>21</v>
@@ -1056,82 +1102,97 @@
         <v>26</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="S8" s="5"/>
-      <c r="T8" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="W8" s="5"/>
-      <c r="X8" s="2" t="s">
-        <v>93</v>
+        <v>48</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="T8" s="5"/>
+      <c r="U8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:25">
       <c r="C9" s="5"/>
       <c r="D9" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="S9" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="T9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="T9" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="W9" s="5"/>
-      <c r="X9" s="2" t="s">
-        <v>94</v>
+      <c r="U9" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="2" t="s">
+        <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:25">
       <c r="C10" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="S10" s="5"/>
-      <c r="T10" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="W10" s="5"/>
-      <c r="X10" s="2" t="s">
-        <v>95</v>
+        <v>50</v>
+      </c>
+      <c r="T10" s="5"/>
+      <c r="U10" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:25">
       <c r="C11" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="S11" s="5"/>
-      <c r="T11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="W11" s="1" t="s">
-        <v>90</v>
+        <v>43</v>
+      </c>
+      <c r="T11" s="5"/>
+      <c r="U11" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
-      <c r="S12" s="1" t="s">
-        <v>71</v>
+    <row r="12" spans="1:25">
+      <c r="C12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25">
+      <c r="C13" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="27">
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C2:C3"/>
@@ -1149,14 +1210,16 @@
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="N1:O1"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="S4:S8"/>
-    <mergeCell ref="S9:S11"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="U3:U5"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="W6:W10"/>
-    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="T4:T8"/>
+    <mergeCell ref="T9:T11"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V3:V5"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="X7:X11"/>
+    <mergeCell ref="X1:Y1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Release 4.2.1: Update Excel files, fixes
</commit_message>
<xml_diff>
--- a/public/excel-files/atlas-matrices.xlsx
+++ b/public/excel-files/atlas-matrices.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="105">
   <si>
     <t>Reconnaissance</t>
   </si>
@@ -100,9 +100,15 @@
     <t>Poison Training Data</t>
   </si>
   <si>
+    <t>Publish Hallucinated Entities</t>
+  </si>
+  <si>
     <t>Publish Poisoned Datasets</t>
   </si>
   <si>
+    <t>Publish Poisoned Models</t>
+  </si>
+  <si>
     <t>Consumer Hardware</t>
   </si>
   <si>
@@ -151,7 +157,7 @@
     <t>Data</t>
   </si>
   <si>
-    <t>GPU Hardware</t>
+    <t>Hardware</t>
   </si>
   <si>
     <t>ML Software</t>
@@ -163,12 +169,12 @@
     <t>Spearphishing via Social Engineering LLM</t>
   </si>
   <si>
+    <t>AI Model Inference API Access</t>
+  </si>
+  <si>
     <t>Full ML Model Access</t>
   </si>
   <si>
-    <t>ML Model Inference API Access</t>
-  </si>
-  <si>
     <t>ML-Enabled Product or Service</t>
   </si>
   <si>
@@ -190,6 +196,9 @@
     <t>Backdoor ML Model</t>
   </si>
   <si>
+    <t>LLM Prompt Self-Replication</t>
+  </si>
+  <si>
     <t>Inject Payload</t>
   </si>
   <si>
@@ -202,6 +211,12 @@
     <t>Unsecured Credentials</t>
   </si>
   <si>
+    <t>Discover AI Model Outputs</t>
+  </si>
+  <si>
+    <t>Discover LLM Hallucinations</t>
+  </si>
+  <si>
     <t>Discover ML Artifacts</t>
   </si>
   <si>
@@ -214,6 +229,12 @@
     <t>LLM Meta Prompt Extraction</t>
   </si>
   <si>
+    <t>Domains</t>
+  </si>
+  <si>
+    <t>Physical Countermeasures</t>
+  </si>
+  <si>
     <t>Data from Information Repositories</t>
   </si>
   <si>
@@ -280,6 +301,9 @@
     <t>Denial of ML Service</t>
   </si>
   <si>
+    <t>Erode Dataset Integrity</t>
+  </si>
+  <si>
     <t>Erode ML Model Integrity</t>
   </si>
   <si>
@@ -287,6 +311,9 @@
   </si>
   <si>
     <t>Spamming ML System with Chaff Data</t>
+  </si>
+  <si>
+    <t>Malicious Package</t>
   </si>
   <si>
     <t>Financial Harm</t>
@@ -697,7 +724,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X12"/>
+  <dimension ref="A1:Y13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -718,17 +745,20 @@
     <col min="13" max="13" width="20.7109375" style="2" customWidth="1"/>
     <col min="14" max="14" width="20.7109375" style="1" customWidth="1"/>
     <col min="15" max="15" width="20.7109375" style="2" customWidth="1"/>
-    <col min="16" max="18" width="20.7109375" customWidth="1"/>
-    <col min="19" max="19" width="20.7109375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="20.7109375" style="2" customWidth="1"/>
-    <col min="21" max="21" width="20.7109375" style="1" customWidth="1"/>
-    <col min="22" max="22" width="20.7109375" style="2" customWidth="1"/>
-    <col min="23" max="23" width="20.7109375" style="1" customWidth="1"/>
-    <col min="24" max="24" width="20.7109375" style="2" customWidth="1"/>
-    <col min="25" max="25" width="20.7109375" customWidth="1"/>
+    <col min="16" max="16" width="20.7109375" customWidth="1"/>
+    <col min="17" max="17" width="20.7109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="20.7109375" style="2" customWidth="1"/>
+    <col min="19" max="19" width="20.7109375" customWidth="1"/>
+    <col min="20" max="20" width="20.7109375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="20.7109375" style="2" customWidth="1"/>
+    <col min="22" max="22" width="20.7109375" style="1" customWidth="1"/>
+    <col min="23" max="23" width="20.7109375" style="2" customWidth="1"/>
+    <col min="24" max="24" width="20.7109375" style="1" customWidth="1"/>
+    <col min="25" max="25" width="20.7109375" style="2" customWidth="1"/>
+    <col min="26" max="26" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -763,26 +793,27 @@
       <c r="P1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3"/>
+      <c r="S1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="3"/>
+      <c r="V1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="3"/>
+      <c r="X1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:25">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -790,99 +821,102 @@
         <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="P2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="S2" t="s">
+        <v>73</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="U2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="Q2" t="s">
-        <v>62</v>
-      </c>
-      <c r="R2" t="s">
-        <v>66</v>
-      </c>
-      <c r="S2" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>86</v>
+      <c r="V2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:25">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="J3" s="5"/>
       <c r="K3" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q3" t="s">
         <v>63</v>
       </c>
-      <c r="R3" t="s">
-        <v>67</v>
-      </c>
-      <c r="S3" s="5"/>
-      <c r="T3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="U3" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>87</v>
+      <c r="Q3" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="S3" t="s">
+        <v>74</v>
+      </c>
+      <c r="T3" s="5"/>
+      <c r="U3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:25">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -890,104 +924,108 @@
         <v>23</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>64</v>
-      </c>
-      <c r="R4" t="s">
-        <v>68</v>
-      </c>
-      <c r="S4" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="T4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U4" s="5"/>
-      <c r="V4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>88</v>
+      <c r="S4" t="s">
+        <v>75</v>
+      </c>
+      <c r="T4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V4" s="5"/>
+      <c r="W4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:25">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="L5" s="5"/>
       <c r="M5" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N5" s="5"/>
       <c r="O5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>65</v>
-      </c>
-      <c r="S5" s="5"/>
-      <c r="T5" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="U5" s="5"/>
-      <c r="V5" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="T5" s="5"/>
+      <c r="U5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="V5" s="5"/>
+      <c r="W5" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:25">
       <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
@@ -998,32 +1036,32 @@
         <v>24</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S6" s="5"/>
-      <c r="T6" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="W6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="T6" s="5"/>
+      <c r="U6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="V6" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="X6" s="2" t="s">
-        <v>91</v>
+      <c r="X6" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:25">
       <c r="A7" s="5"/>
       <c r="B7" s="2" t="s">
         <v>20</v>
@@ -1033,21 +1071,29 @@
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="S7" s="5"/>
-      <c r="T7" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="W7" s="5"/>
-      <c r="X7" s="2" t="s">
-        <v>92</v>
+        <v>47</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="T7" s="5"/>
+      <c r="U7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="X7" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:25">
       <c r="A8" s="5"/>
       <c r="B8" s="2" t="s">
         <v>21</v>
@@ -1056,82 +1102,97 @@
         <v>26</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="S8" s="5"/>
-      <c r="T8" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="W8" s="5"/>
-      <c r="X8" s="2" t="s">
-        <v>93</v>
+        <v>48</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="T8" s="5"/>
+      <c r="U8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:25">
       <c r="C9" s="5"/>
       <c r="D9" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="S9" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="T9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="T9" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="W9" s="5"/>
-      <c r="X9" s="2" t="s">
-        <v>94</v>
+      <c r="U9" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="2" t="s">
+        <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:25">
       <c r="C10" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="S10" s="5"/>
-      <c r="T10" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="W10" s="5"/>
-      <c r="X10" s="2" t="s">
-        <v>95</v>
+        <v>50</v>
+      </c>
+      <c r="T10" s="5"/>
+      <c r="U10" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:25">
       <c r="C11" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="S11" s="5"/>
-      <c r="T11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="W11" s="1" t="s">
-        <v>90</v>
+        <v>43</v>
+      </c>
+      <c r="T11" s="5"/>
+      <c r="U11" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
-      <c r="S12" s="1" t="s">
-        <v>71</v>
+    <row r="12" spans="1:25">
+      <c r="C12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25">
+      <c r="C13" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="27">
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C2:C3"/>
@@ -1149,14 +1210,16 @@
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="N1:O1"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="S4:S8"/>
-    <mergeCell ref="S9:S11"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="U3:U5"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="W6:W10"/>
-    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="T4:T8"/>
+    <mergeCell ref="T9:T11"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V3:V5"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="X7:X11"/>
+    <mergeCell ref="X1:Y1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Release 4.3.0: update to atlas-data 4.8.0
</commit_message>
<xml_diff>
--- a/public/excel-files/atlas-matrices.xlsx
+++ b/public/excel-files/atlas-matrices.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="118">
   <si>
     <t>Reconnaissance</t>
   </si>
@@ -61,6 +61,9 @@
     <t>Active Scanning</t>
   </si>
   <si>
+    <t>Gather RAG-Indexed Targets</t>
+  </si>
+  <si>
     <t>Search Application Repositories</t>
   </si>
   <si>
@@ -94,6 +97,9 @@
     <t>Establish Accounts</t>
   </si>
   <si>
+    <t>LLM Prompt Crafting</t>
+  </si>
+  <si>
     <t>Obtain Capabilities</t>
   </si>
   <si>
@@ -109,6 +115,9 @@
     <t>Publish Poisoned Models</t>
   </si>
   <si>
+    <t>Retrieval Content Crafting</t>
+  </si>
+  <si>
     <t>Consumer Hardware</t>
   </si>
   <si>
@@ -136,16 +145,52 @@
     <t>Exploit Public-Facing Application</t>
   </si>
   <si>
+    <t>ML Supply Chain Compromise</t>
+  </si>
+  <si>
+    <t>Phishing</t>
+  </si>
+  <si>
+    <t>Valid Accounts</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Hardware</t>
+  </si>
+  <si>
+    <t>ML Software</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Spearphishing via Social Engineering LLM</t>
+  </si>
+  <si>
+    <t>AI Model Inference API Access</t>
+  </si>
+  <si>
+    <t>Full ML Model Access</t>
+  </si>
+  <si>
+    <t>ML-Enabled Product or Service</t>
+  </si>
+  <si>
+    <t>Physical Environment Access</t>
+  </si>
+  <si>
+    <t>Command and Scripting Interpreter</t>
+  </si>
+  <si>
+    <t>LLM Plugin Compromise</t>
+  </si>
+  <si>
     <t>LLM Prompt Injection</t>
   </si>
   <si>
-    <t>ML Supply Chain Compromise</t>
-  </si>
-  <si>
-    <t>Phishing</t>
-  </si>
-  <si>
-    <t>Valid Accounts</t>
+    <t>User Execution</t>
   </si>
   <si>
     <t>Direct</t>
@@ -154,42 +199,6 @@
     <t>Indirect</t>
   </si>
   <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>Hardware</t>
-  </si>
-  <si>
-    <t>ML Software</t>
-  </si>
-  <si>
-    <t>Model</t>
-  </si>
-  <si>
-    <t>Spearphishing via Social Engineering LLM</t>
-  </si>
-  <si>
-    <t>AI Model Inference API Access</t>
-  </si>
-  <si>
-    <t>Full ML Model Access</t>
-  </si>
-  <si>
-    <t>ML-Enabled Product or Service</t>
-  </si>
-  <si>
-    <t>Physical Environment Access</t>
-  </si>
-  <si>
-    <t>Command and Scripting Interpreter</t>
-  </si>
-  <si>
-    <t>LLM Plugin Compromise</t>
-  </si>
-  <si>
-    <t>User Execution</t>
-  </si>
-  <si>
     <t>Unsafe ML Artifacts</t>
   </si>
   <si>
@@ -199,6 +208,9 @@
     <t>LLM Prompt Self-Replication</t>
   </si>
   <si>
+    <t>RAG Poisoning</t>
+  </si>
+  <si>
     <t>Inject Payload</t>
   </si>
   <si>
@@ -208,6 +220,18 @@
     <t>LLM Jailbreak</t>
   </si>
   <si>
+    <t>False RAG Entry Injection</t>
+  </si>
+  <si>
+    <t>LLM Prompt Obfuscation</t>
+  </si>
+  <si>
+    <t>LLM Trusted Output Components Manipulation</t>
+  </si>
+  <si>
+    <t>Citations</t>
+  </si>
+  <si>
     <t>Unsecured Credentials</t>
   </si>
   <si>
@@ -217,6 +241,9 @@
     <t>Discover LLM Hallucinations</t>
   </si>
   <si>
+    <t>Discover LLM System Information</t>
+  </si>
+  <si>
     <t>Discover ML Artifacts</t>
   </si>
   <si>
@@ -226,7 +253,7 @@
     <t>Discover ML Model Ontology</t>
   </si>
   <si>
-    <t>LLM Meta Prompt Extraction</t>
+    <t>Generative AI</t>
   </si>
   <si>
     <t>Domains</t>
@@ -235,6 +262,15 @@
     <t>Physical Countermeasures</t>
   </si>
   <si>
+    <t>Special Character Sets</t>
+  </si>
+  <si>
+    <t>System Instruction Keywords</t>
+  </si>
+  <si>
+    <t>System Prompt</t>
+  </si>
+  <si>
     <t>Data from Information Repositories</t>
   </si>
   <si>
@@ -281,6 +317,9 @@
   </si>
   <si>
     <t>Exfiltration via ML Inference API</t>
+  </si>
+  <si>
+    <t>Extract LLM System Prompt</t>
   </si>
   <si>
     <t>LLM Data Leakage</t>
@@ -724,7 +763,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y13"/>
+  <dimension ref="A1:X15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -741,24 +780,23 @@
     <col min="9" max="9" width="20.7109375" style="2" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" style="1" customWidth="1"/>
     <col min="11" max="11" width="20.7109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="20.7109375" style="2" customWidth="1"/>
-    <col min="14" max="14" width="20.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="20.7109375" style="2" customWidth="1"/>
-    <col min="16" max="16" width="20.7109375" customWidth="1"/>
-    <col min="17" max="17" width="20.7109375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="20.7109375" style="2" customWidth="1"/>
-    <col min="19" max="19" width="20.7109375" customWidth="1"/>
-    <col min="20" max="20" width="20.7109375" style="1" customWidth="1"/>
-    <col min="21" max="21" width="20.7109375" style="2" customWidth="1"/>
-    <col min="22" max="22" width="20.7109375" style="1" customWidth="1"/>
-    <col min="23" max="23" width="20.7109375" style="2" customWidth="1"/>
-    <col min="24" max="24" width="20.7109375" style="1" customWidth="1"/>
-    <col min="25" max="25" width="20.7109375" style="2" customWidth="1"/>
-    <col min="26" max="26" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="20.7109375" style="2" customWidth="1"/>
+    <col min="15" max="15" width="20.7109375" customWidth="1"/>
+    <col min="16" max="16" width="20.7109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="20.7109375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="20.7109375" customWidth="1"/>
+    <col min="19" max="19" width="20.7109375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="20.7109375" style="2" customWidth="1"/>
+    <col min="21" max="21" width="20.7109375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="20.7109375" style="2" customWidth="1"/>
+    <col min="23" max="23" width="20.7109375" style="1" customWidth="1"/>
+    <col min="24" max="24" width="20.7109375" style="2" customWidth="1"/>
+    <col min="25" max="25" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:24">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -782,49 +820,48 @@
         <v>5</v>
       </c>
       <c r="K1" s="3"/>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="3"/>
-      <c r="P1" s="4" t="s">
+      <c r="N1" s="3"/>
+      <c r="O1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="3"/>
-      <c r="S1" s="4" t="s">
+      <c r="Q1" s="3"/>
+      <c r="R1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3" t="s">
+      <c r="T1" s="3"/>
+      <c r="U1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3" t="s">
+      <c r="V1" s="3"/>
+      <c r="W1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="Y1" s="3"/>
-    </row>
-    <row r="2" spans="1:25">
+      <c r="X1" s="3"/>
+    </row>
+    <row r="2" spans="1:24">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G2" t="s">
         <v>51</v>
@@ -833,49 +870,52 @@
         <v>55</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="P2" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="S2" t="s">
+      <c r="L2" t="s">
+        <v>67</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O2" t="s">
+        <v>72</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="T2" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25">
+      <c r="Q2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="R2" t="s">
+        <v>85</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G3" t="s">
         <v>52</v>
@@ -885,341 +925,347 @@
       </c>
       <c r="J3" s="5"/>
       <c r="K3" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="L3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L3" t="s">
         <v>56</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q3" s="5" t="s">
+      <c r="M3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R3" t="s">
+        <v>86</v>
+      </c>
+      <c r="S3" s="5"/>
+      <c r="T3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="R3" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="S3" t="s">
-        <v>74</v>
-      </c>
-      <c r="T3" s="5"/>
-      <c r="U3" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="V3" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25">
+      <c r="U3" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G4" t="s">
         <v>53</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="5" t="s">
         <v>57</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="S4" t="s">
-        <v>75</v>
-      </c>
-      <c r="T4" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="V4" s="5"/>
-      <c r="W4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="R4" t="s">
+        <v>87</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="T4" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="X4" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="Y4" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25">
+      <c r="U4" s="5"/>
+      <c r="V4" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G5" t="s">
         <v>54</v>
       </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="L5" s="5"/>
-      <c r="M5" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="N5" s="5"/>
-      <c r="O5" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="T5" s="5"/>
-      <c r="U5" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="V5" s="5"/>
-      <c r="W5" s="2" t="s">
+      <c r="H5" s="5"/>
+      <c r="I5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="S5" s="5"/>
+      <c r="T5" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="X5" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25">
-      <c r="A6" s="5" t="s">
+      <c r="U5" s="5"/>
+      <c r="V5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
+      <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="S6" s="5"/>
+      <c r="T6" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
+      <c r="A7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="T6" s="5"/>
-      <c r="U6" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="V6" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="X6" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25">
-      <c r="A7" s="5"/>
       <c r="B7" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="T7" s="5"/>
-      <c r="U7" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="X7" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="Y7" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25">
+        <v>49</v>
+      </c>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="S7" s="5"/>
+      <c r="T7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="W7" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
       <c r="A8" s="5"/>
       <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="5"/>
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="F8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="T8" s="5"/>
-      <c r="U8" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="X8" s="5"/>
-      <c r="Y8" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25">
-      <c r="C9" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="S8" s="5"/>
+      <c r="T8" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="W8" s="5"/>
+      <c r="X8" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
+      <c r="A9" s="5"/>
+      <c r="B9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="D9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="T9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P9" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="U9" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="X9" s="5"/>
-      <c r="Y9" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25">
-      <c r="C10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="T10" s="5"/>
-      <c r="U10" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="X10" s="5"/>
-      <c r="Y10" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25">
+      <c r="S9" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="W9" s="5"/>
+      <c r="X9" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
+      <c r="C10" s="5"/>
+      <c r="D10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="S10" s="5"/>
+      <c r="T10" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="W10" s="5"/>
+      <c r="X10" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24">
       <c r="C11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T11" s="5"/>
-      <c r="U11" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="X11" s="5"/>
-      <c r="Y11" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25">
+        <v>29</v>
+      </c>
+      <c r="S11" s="5"/>
+      <c r="T11" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="W11" s="5"/>
+      <c r="X11" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24">
       <c r="C12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T12" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="X12" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25">
+        <v>30</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24">
       <c r="C13" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24">
+      <c r="C14" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24">
+      <c r="C15" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="A6:A8"/>
+  <mergeCells count="24">
+    <mergeCell ref="A7:A9"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C9:C10"/>
     <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="E4:E7"/>
     <mergeCell ref="E1:F1"/>
+    <mergeCell ref="H4:H5"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J2:J3"/>
-    <mergeCell ref="J4:J5"/>
     <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="T4:T8"/>
-    <mergeCell ref="T9:T11"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V3:V5"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="X7:X11"/>
-    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="P5:P7"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="S4:S8"/>
+    <mergeCell ref="S9:S11"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="U3:U5"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="W7:W11"/>
+    <mergeCell ref="W1:X1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Release 4.4.0: update to atlas-data 4.9.0, update articles
</commit_message>
<xml_diff>
--- a/public/excel-files/atlas-matrices.xlsx
+++ b/public/excel-files/atlas-matrices.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="130">
   <si>
     <t>Reconnaissance</t>
   </si>
@@ -25,7 +25,7 @@
     <t>Initial Access</t>
   </si>
   <si>
-    <t>ML Model Access</t>
+    <t>AI Model Access</t>
   </si>
   <si>
     <t>Execution</t>
@@ -49,7 +49,10 @@
     <t>Collection</t>
   </si>
   <si>
-    <t>ML Attack Staging</t>
+    <t>AI Attack Staging</t>
+  </si>
+  <si>
+    <t>Command and Control</t>
   </si>
   <si>
     <t>Exfiltration</t>
@@ -67,15 +70,15 @@
     <t>Search Application Repositories</t>
   </si>
   <si>
+    <t>Search Open AI Vulnerability Analysis</t>
+  </si>
+  <si>
+    <t>Search Open Technical Databases</t>
+  </si>
+  <si>
     <t>Search Victim-Owned Websites</t>
   </si>
   <si>
-    <t>Search for Publicly Available Adversarial Vulnerability Analysis</t>
-  </si>
-  <si>
-    <t>Search for Victim's Publicly Available Research Materials</t>
-  </si>
-  <si>
     <t>Journals and Conference Proceedings</t>
   </si>
   <si>
@@ -88,7 +91,7 @@
     <t>Acquire Infrastructure</t>
   </si>
   <si>
-    <t>Acquire Public ML Artifacts</t>
+    <t>Acquire Public AI Artifacts</t>
   </si>
   <si>
     <t>Develop Capabilities</t>
@@ -118,51 +121,57 @@
     <t>Retrieval Content Crafting</t>
   </si>
   <si>
+    <t>Stage Capabilities</t>
+  </si>
+  <si>
+    <t>AI Development Workspaces</t>
+  </si>
+  <si>
     <t>Consumer Hardware</t>
   </si>
   <si>
-    <t>ML Development Workspaces</t>
-  </si>
-  <si>
     <t>Datasets</t>
   </si>
   <si>
     <t>Models</t>
   </si>
   <si>
-    <t>Adversarial ML Attacks</t>
-  </si>
-  <si>
-    <t>Adversarial ML Attack Implementations</t>
+    <t>Adversarial AI Attacks</t>
+  </si>
+  <si>
+    <t>Adversarial AI Attack Implementations</t>
   </si>
   <si>
     <t>Software Tools</t>
   </si>
   <si>
-    <t>Evade ML Model</t>
+    <t>AI Supply Chain Compromise</t>
+  </si>
+  <si>
+    <t>Drive-by Compromise</t>
+  </si>
+  <si>
+    <t>Evade AI Model</t>
   </si>
   <si>
     <t>Exploit Public-Facing Application</t>
   </si>
   <si>
-    <t>ML Supply Chain Compromise</t>
-  </si>
-  <si>
     <t>Phishing</t>
   </si>
   <si>
     <t>Valid Accounts</t>
   </si>
   <si>
+    <t>AI Software</t>
+  </si>
+  <si>
     <t>Data</t>
   </si>
   <si>
     <t>Hardware</t>
   </si>
   <si>
-    <t>ML Software</t>
-  </si>
-  <si>
     <t>Model</t>
   </si>
   <si>
@@ -172,10 +181,10 @@
     <t>AI Model Inference API Access</t>
   </si>
   <si>
-    <t>Full ML Model Access</t>
-  </si>
-  <si>
-    <t>ML-Enabled Product or Service</t>
+    <t>AI-Enabled Product or Service</t>
+  </si>
+  <si>
+    <t>Full AI Model Access</t>
   </si>
   <si>
     <t>Physical Environment Access</t>
@@ -199,42 +208,69 @@
     <t>Indirect</t>
   </si>
   <si>
-    <t>Unsafe ML Artifacts</t>
-  </si>
-  <si>
-    <t>Backdoor ML Model</t>
+    <t>Unsafe AI Artifacts</t>
   </si>
   <si>
     <t>LLM Prompt Self-Replication</t>
   </si>
   <si>
+    <t>Manipulate AI Model</t>
+  </si>
+  <si>
     <t>RAG Poisoning</t>
   </si>
   <si>
-    <t>Inject Payload</t>
-  </si>
-  <si>
-    <t>Poison ML Model</t>
+    <t>Modify AI Model Architecture</t>
+  </si>
+  <si>
+    <t>Poison AI Model</t>
   </si>
   <si>
     <t>LLM Jailbreak</t>
   </si>
   <si>
+    <t>Corrupt AI Model</t>
+  </si>
+  <si>
     <t>False RAG Entry Injection</t>
   </si>
   <si>
+    <t>Impersonation</t>
+  </si>
+  <si>
     <t>LLM Prompt Obfuscation</t>
   </si>
   <si>
     <t>LLM Trusted Output Components Manipulation</t>
   </si>
   <si>
+    <t>Masquerading</t>
+  </si>
+  <si>
     <t>Citations</t>
   </si>
   <si>
+    <t>Container Registry</t>
+  </si>
+  <si>
+    <t>Embed Malware</t>
+  </si>
+  <si>
     <t>Unsecured Credentials</t>
   </si>
   <si>
+    <t>Cloud Service Discovery</t>
+  </si>
+  <si>
+    <t>Discover AI Artifacts</t>
+  </si>
+  <si>
+    <t>Discover AI Model Family</t>
+  </si>
+  <si>
+    <t>Discover AI Model Ontology</t>
+  </si>
+  <si>
     <t>Discover AI Model Outputs</t>
   </si>
   <si>
@@ -244,15 +280,6 @@
     <t>Discover LLM System Information</t>
   </si>
   <si>
-    <t>Discover ML Artifacts</t>
-  </si>
-  <si>
-    <t>Discover ML Model Family</t>
-  </si>
-  <si>
-    <t>Discover ML Model Ontology</t>
-  </si>
-  <si>
     <t>Generative AI</t>
   </si>
   <si>
@@ -271,19 +298,19 @@
     <t>System Prompt</t>
   </si>
   <si>
+    <t>AI Artifact Collection</t>
+  </si>
+  <si>
     <t>Data from Information Repositories</t>
   </si>
   <si>
     <t>Data from Local System</t>
   </si>
   <si>
-    <t>ML Artifact Collection</t>
-  </si>
-  <si>
     <t>Craft Adversarial Data</t>
   </si>
   <si>
-    <t>Create Proxy ML Model</t>
+    <t>Create Proxy AI Model</t>
   </si>
   <si>
     <t>Verify Attack</t>
@@ -304,7 +331,7 @@
     <t>White-Box Optimization</t>
   </si>
   <si>
-    <t>Train Proxy via Gathered ML Artifacts</t>
+    <t>Train Proxy via Gathered AI Artifacts</t>
   </si>
   <si>
     <t>Train Proxy via Replication</t>
@@ -313,52 +340,61 @@
     <t>Use Pre-Trained Model</t>
   </si>
   <si>
+    <t>Reverse Shell</t>
+  </si>
+  <si>
+    <t>Exfiltration via AI Inference API</t>
+  </si>
+  <si>
     <t>Exfiltration via Cyber Means</t>
   </si>
   <si>
-    <t>Exfiltration via ML Inference API</t>
-  </si>
-  <si>
     <t>Extract LLM System Prompt</t>
   </si>
   <si>
     <t>LLM Data Leakage</t>
   </si>
   <si>
-    <t>Extract ML Model</t>
+    <t>LLM Response Rendering</t>
+  </si>
+  <si>
+    <t>Extract AI Model</t>
   </si>
   <si>
     <t>Infer Training Data Membership</t>
   </si>
   <si>
-    <t>Invert ML Model</t>
+    <t>Invert AI Model</t>
+  </si>
+  <si>
+    <t>Serverless</t>
   </si>
   <si>
     <t>Cost Harvesting</t>
   </si>
   <si>
-    <t>Denial of ML Service</t>
+    <t>Denial of AI Service</t>
+  </si>
+  <si>
+    <t>Erode AI Model Integrity</t>
   </si>
   <si>
     <t>Erode Dataset Integrity</t>
   </si>
   <si>
-    <t>Erode ML Model Integrity</t>
-  </si>
-  <si>
     <t>External Harms</t>
   </si>
   <si>
-    <t>Spamming ML System with Chaff Data</t>
+    <t>Spamming AI System with Chaff Data</t>
   </si>
   <si>
     <t>Malicious Package</t>
   </si>
   <si>
+    <t>AI Intellectual Property Theft</t>
+  </si>
+  <si>
     <t>Financial Harm</t>
-  </si>
-  <si>
-    <t>ML Intellectual Property Theft</t>
   </si>
   <si>
     <t>Reputational Harm</t>
@@ -763,7 +799,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X15"/>
+  <dimension ref="A1:Y16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -789,14 +825,15 @@
     <col min="18" max="18" width="20.7109375" customWidth="1"/>
     <col min="19" max="19" width="20.7109375" style="1" customWidth="1"/>
     <col min="20" max="20" width="20.7109375" style="2" customWidth="1"/>
-    <col min="21" max="21" width="20.7109375" style="1" customWidth="1"/>
-    <col min="22" max="22" width="20.7109375" style="2" customWidth="1"/>
-    <col min="23" max="23" width="20.7109375" style="1" customWidth="1"/>
-    <col min="24" max="24" width="20.7109375" style="2" customWidth="1"/>
-    <col min="25" max="25" width="20.7109375" customWidth="1"/>
+    <col min="21" max="21" width="20.7109375" customWidth="1"/>
+    <col min="22" max="22" width="20.7109375" style="1" customWidth="1"/>
+    <col min="23" max="23" width="20.7109375" style="2" customWidth="1"/>
+    <col min="24" max="24" width="20.7109375" style="1" customWidth="1"/>
+    <col min="25" max="25" width="20.7109375" style="2" customWidth="1"/>
+    <col min="26" max="26" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -841,431 +878,472 @@
         <v>11</v>
       </c>
       <c r="T1" s="3"/>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="X1" s="3"/>
-    </row>
-    <row r="2" spans="1:24">
+      <c r="W1" s="3"/>
+      <c r="X1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y1" s="3"/>
+    </row>
+    <row r="2" spans="1:25">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="G2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="K2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>65</v>
       </c>
       <c r="L2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="O2" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="R2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24">
+        <v>100</v>
+      </c>
+      <c r="U2" t="s">
+        <v>108</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="G3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J3" s="5"/>
+        <v>59</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="K3" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>80</v>
+        <v>45</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="R3" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="S3" s="5"/>
       <c r="T3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="U3" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24">
+        <v>101</v>
+      </c>
+      <c r="V3" s="5"/>
+      <c r="W3" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>43</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E4" s="5"/>
       <c r="F4" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="2" t="s">
-        <v>81</v>
+        <v>62</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="K4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="R4" t="s">
-        <v>87</v>
-      </c>
-      <c r="S4" s="5" t="s">
-        <v>88</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="S4" s="5"/>
       <c r="T4" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="U4" s="5"/>
-      <c r="V4" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="X4" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24">
+        <v>102</v>
+      </c>
+      <c r="V4" s="5"/>
+      <c r="W4" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="P5" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>82</v>
+        <v>30</v>
+      </c>
+      <c r="M5" s="5"/>
+      <c r="N5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="S5" s="5"/>
       <c r="T5" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="U5" s="5"/>
-      <c r="V5" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24">
-      <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>103</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25">
+      <c r="A6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="P6" s="5"/>
+        <v>67</v>
+      </c>
+      <c r="M6" s="5"/>
+      <c r="N6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="Q6" s="2" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="S6" s="5"/>
       <c r="T6" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="W6" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24">
-      <c r="A7" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25">
+      <c r="A7" s="5"/>
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="P7" s="5"/>
+        <v>27</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>86</v>
+      </c>
       <c r="Q7" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="S7" s="5"/>
+        <v>89</v>
+      </c>
+      <c r="S7" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="T7" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="W7" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="X7" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24">
+        <v>105</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="X7" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25">
       <c r="A8" s="5"/>
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>76</v>
+        <v>46</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="S8" s="5"/>
       <c r="T8" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="W8" s="5"/>
-      <c r="X8" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24">
-      <c r="A9" s="5"/>
-      <c r="B9" s="2" t="s">
-        <v>22</v>
+        <v>106</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="S9" s="5" t="s">
-        <v>89</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="S9" s="5"/>
       <c r="T9" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="W9" s="5"/>
-      <c r="X9" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24">
+        <v>107</v>
+      </c>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25">
       <c r="C10" s="5"/>
       <c r="D10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="S10" s="5"/>
+        <v>42</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="S10" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="T10" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="W10" s="5"/>
-      <c r="X10" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24">
+        <v>68</v>
+      </c>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25">
       <c r="C11" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="S11" s="5"/>
       <c r="T11" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="W11" s="5"/>
-      <c r="X11" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24">
+        <v>69</v>
+      </c>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25">
       <c r="C12" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="W12" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24">
+        <v>99</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25">
       <c r="C13" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25">
       <c r="C14" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25">
       <c r="C15" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25">
+      <c r="C16" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="A7:A9"/>
+  <mergeCells count="25">
+    <mergeCell ref="A6:A8"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E4:E7"/>
+    <mergeCell ref="E2:E5"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="J3:J4"/>
     <mergeCell ref="J1:K1"/>
+    <mergeCell ref="M4:M6"/>
     <mergeCell ref="M1:N1"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="P5:P7"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="P9:P11"/>
     <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="S4:S8"/>
-    <mergeCell ref="S9:S11"/>
+    <mergeCell ref="S2:S6"/>
+    <mergeCell ref="S7:S9"/>
+    <mergeCell ref="S10:S11"/>
     <mergeCell ref="S1:T1"/>
-    <mergeCell ref="U3:U5"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="W7:W11"/>
-    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="V2:V4"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="X7:X11"/>
+    <mergeCell ref="X1:Y1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>